<commit_message>
Corrected mistake in BOM
</commit_message>
<xml_diff>
--- a/Hardware/Veno-Echo BOM.xlsx
+++ b/Hardware/Veno-Echo BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/venuslee/Documents/Venus Instruments/Veno-Echo external/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamfulford/Documents/Veno-Echo/Hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98F176A-0AC4-B74A-B5D1-A7A0B7522599}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3648E9-D272-C14B-9803-B2DCECDB744F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{599F4D57-485E-EE44-8FF2-78268A418B88}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="37560" windowHeight="21140" xr2:uid="{599F4D57-485E-EE44-8FF2-78268A418B88}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1041,7 +1041,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1690,7 +1690,7 @@
     </row>
     <row r="26" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>171</v>

</xml_diff>

<commit_message>
Added part numbers to 20pin sockets
</commit_message>
<xml_diff>
--- a/Hardware/Veno-Echo BOM.xlsx
+++ b/Hardware/Veno-Echo BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamfulford/Documents/Veno-Echo/Hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA42AE73-19C7-B74D-B444-80864A3A2C45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C704C0E9-FD84-1648-B129-94B294C1A9B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{599F4D57-485E-EE44-8FF2-78268A418B88}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="189">
   <si>
     <t>Qty</t>
   </si>
@@ -595,6 +595,12 @@
   </si>
   <si>
     <t>mono Thonkiconn</t>
+  </si>
+  <si>
+    <t>200-SSW12001GS</t>
+  </si>
+  <si>
+    <t>SAM1209-20-ND</t>
   </si>
 </sst>
 </file>
@@ -1040,8 +1046,8 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
+      <pane ySplit="3" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1707,8 +1713,12 @@
       <c r="F26" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
+      <c r="G26" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>187</v>
+      </c>
       <c r="I26" s="7"/>
     </row>
     <row r="27" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Sorted components by SMD and TH
</commit_message>
<xml_diff>
--- a/Hardware/Veno-Echo BOM.xlsx
+++ b/Hardware/Veno-Echo BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamfulford/Documents/Veno-Echo/Hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C704C0E9-FD84-1648-B129-94B294C1A9B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{33339A64-E898-E845-9E32-6EE9081A12C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{599F4D57-485E-EE44-8FF2-78268A418B88}"/>
+    <workbookView xWindow="2840" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{599F4D57-485E-EE44-8FF2-78268A418B88}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="188">
   <si>
     <t>Qty</t>
   </si>
@@ -582,25 +582,22 @@
     <t>20 Pin Female header sockets</t>
   </si>
   <si>
-    <t>20 pin socket</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
-    <t>20 Pin Female header socket</t>
-  </si>
-  <si>
     <t xml:space="preserve"> PJ301M-12 / PJ398SM</t>
   </si>
   <si>
-    <t>mono Thonkiconn</t>
-  </si>
-  <si>
     <t>200-SSW12001GS</t>
   </si>
   <si>
     <t>SAM1209-20-ND</t>
+  </si>
+  <si>
+    <t>20 pin header socket (optional)</t>
+  </si>
+  <si>
+    <t>mono Thonkiconn (3 leg)</t>
   </si>
 </sst>
 </file>
@@ -654,7 +651,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -664,6 +661,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -696,7 +699,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -727,6 +730,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1046,8 +1052,8 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1107,698 +1113,704 @@
       </c>
     </row>
     <row r="4" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
+      <c r="A4" s="11">
+        <v>5</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="11">
+        <v>7</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="I5" s="11"/>
+    </row>
+    <row r="6" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="11">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B6" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="I6" s="11"/>
+    </row>
+    <row r="7" spans="1:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="11">
+        <v>14</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="I7" s="11"/>
+    </row>
+    <row r="8" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="11">
+        <v>6</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="I8" s="11"/>
+    </row>
+    <row r="9" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="11">
+        <v>2</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="I9" s="11"/>
+    </row>
+    <row r="10" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="11">
+        <v>2</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="I10" s="11"/>
+    </row>
+    <row r="11" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="11">
+        <v>4</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="I11" s="11"/>
+    </row>
+    <row r="12" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="11">
+        <v>2</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="I12" s="11"/>
+    </row>
+    <row r="13" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="11">
+        <v>1</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="I13" s="11"/>
+    </row>
+    <row r="14" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="11">
+        <v>1</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="I14" s="11"/>
+    </row>
+    <row r="15" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="11">
+        <v>1</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="I15" s="11"/>
+    </row>
+    <row r="16" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="11">
         <v>3</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="I4" s="7"/>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="7">
+      <c r="B16" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="I16" s="11"/>
+    </row>
+    <row r="17" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="11">
         <v>1</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="B17" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="I17" s="11"/>
+    </row>
+    <row r="18" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="11">
         <v>4</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="I5" s="7"/>
-    </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="7">
-        <v>1</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="D6" s="7" t="s">
+      <c r="B18" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="I18" s="11"/>
+    </row>
+    <row r="19" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="11">
+        <v>7</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="I19" s="11"/>
+    </row>
+    <row r="20" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="11">
+        <v>7</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="I20" s="11"/>
+    </row>
+    <row r="21" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="11">
+        <v>3</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="I21" s="11"/>
+    </row>
+    <row r="22" spans="1:9" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A22" s="11">
+        <v>27</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="I22" s="11"/>
+    </row>
+    <row r="23" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="11">
+        <v>3</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="I23" s="11"/>
+    </row>
+    <row r="24" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="11">
         <v>4</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="I6" s="7"/>
-    </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
+      <c r="B24" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="I24" s="11"/>
+    </row>
+    <row r="25" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="11">
+        <v>7</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="I25" s="11"/>
+    </row>
+    <row r="26" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="11">
+        <v>2</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="I26" s="11"/>
+    </row>
+    <row r="27" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="11">
         <v>3</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
-        <v>27</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="7">
-        <v>14</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="I9" s="7"/>
-    </row>
-    <row r="10" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="7">
-        <v>4</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="I10" s="7"/>
-    </row>
-    <row r="11" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="7">
-        <v>4</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="I11" s="7"/>
-    </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="7">
-        <v>7</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="I12" s="7"/>
-    </row>
-    <row r="13" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="7">
-        <v>5</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="I13" s="7"/>
-    </row>
-    <row r="14" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="7">
-        <v>3</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="7">
+      <c r="B27" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="I27" s="11"/>
+    </row>
+    <row r="28" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="11">
         <v>2</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="I15" s="7"/>
-    </row>
-    <row r="16" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="7">
-        <v>7</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="I16" s="7"/>
-    </row>
-    <row r="17" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="7">
-        <v>2</v>
-      </c>
-      <c r="B17" s="7" t="s">
+      <c r="B28" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C28" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D28" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E28" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="F17" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="G17" s="7" t="s">
+      <c r="F28" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G28" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="H28" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="I17" s="7"/>
-    </row>
-    <row r="18" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="7">
-        <v>1</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="I18" s="7"/>
-    </row>
-    <row r="19" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="7">
-        <v>7</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="I19" s="7"/>
-    </row>
-    <row r="20" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="7">
-        <v>2</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="I20" s="7"/>
-    </row>
-    <row r="21" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="7">
-        <v>6</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="I21" s="7"/>
-    </row>
-    <row r="22" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="7">
-        <v>2</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="I22" s="7"/>
-    </row>
-    <row r="23" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="7">
-        <v>7</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="I23" s="7"/>
-    </row>
-    <row r="24" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="7">
-        <v>2</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="I24" s="7"/>
-    </row>
-    <row r="25" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="7">
-        <v>3</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="I25" s="7"/>
-    </row>
-    <row r="26" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="7">
-        <v>2</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="I26" s="7"/>
-    </row>
-    <row r="27" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="7">
-        <v>1</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="I27" s="7"/>
-    </row>
-    <row r="28" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="7">
-        <v>2</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="I28" s="7"/>
+      <c r="I28" s="11"/>
     </row>
     <row r="29" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
+        <v>2</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>65</v>
-      </c>
       <c r="C29" s="7" t="s">
-        <v>63</v>
+        <v>163</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>64</v>
+        <v>164</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>134</v>
+        <v>83</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>135</v>
+        <v>85</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
       <c r="I29" s="7"/>
     </row>
@@ -1807,75 +1819,79 @@
         <v>1</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>66</v>
+        <v>149</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="F30" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>182</v>
+      </c>
       <c r="G30" s="7" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="I30" s="7"/>
     </row>
-    <row r="31" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
+        <v>1</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D31" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>76</v>
-      </c>
       <c r="E31" s="7" t="s">
-        <v>140</v>
+        <v>87</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>179</v>
+        <v>152</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>180</v>
+        <v>154</v>
       </c>
       <c r="I31" s="7"/>
     </row>
     <row r="32" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>74</v>
+        <v>186</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>74</v>
+        <v>168</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F32" s="7"/>
+        <v>181</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>182</v>
+      </c>
       <c r="G32" s="7" t="s">
-        <v>142</v>
+        <v>185</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>143</v>
+        <v>184</v>
       </c>
       <c r="I32" s="7"/>
     </row>
@@ -1884,50 +1900,52 @@
         <v>1</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="F33" s="7"/>
+        <v>137</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>182</v>
+      </c>
       <c r="G33" s="7" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>174</v>
+        <v>139</v>
       </c>
       <c r="I33" s="7"/>
     </row>
     <row r="34" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>72</v>
+        <v>141</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="I34" s="7"/>
     </row>
@@ -1947,7 +1965,9 @@
       <c r="E35" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="F35" s="7"/>
+      <c r="F35" s="7" t="s">
+        <v>182</v>
+      </c>
       <c r="G35" s="7" t="s">
         <v>174</v>
       </c>
@@ -1966,15 +1986,17 @@
         <v>73</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>52</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="F36" s="7"/>
+        <v>187</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>182</v>
+      </c>
       <c r="G36" s="7" t="s">
         <v>174</v>
       </c>
@@ -2001,7 +2023,9 @@
       <c r="E37" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="F37" s="7"/>
+      <c r="F37" s="7" t="s">
+        <v>182</v>
+      </c>
       <c r="G37" s="7" t="s">
         <v>174</v>
       </c>
@@ -2024,7 +2048,9 @@
       <c r="E38" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="F38" s="8"/>
+      <c r="F38" s="8" t="s">
+        <v>182</v>
+      </c>
       <c r="G38" s="7" t="s">
         <v>174</v>
       </c>
@@ -2036,6 +2062,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:I28">
+    <sortCondition ref="B4:B28"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>